<commit_message>
added new EF database
</commit_message>
<xml_diff>
--- a/ResumenPM.xlsx
+++ b/ResumenPM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ignaz/Documents/STEP_3/copert5App/copert_5/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DF1E088-C668-2D4B-BA44-2A1EF74A0AB1}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD7822D0-BF12-B24B-92ED-25B8FBE04776}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -571,7 +571,7 @@
   <dimension ref="A1:V97"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="V42" sqref="V42:V47"/>
+      <selection activeCell="U47" sqref="U47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6163,17 +6163,8 @@
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="C83:C97"/>
-    <mergeCell ref="C42:C49"/>
-    <mergeCell ref="C50:C55"/>
-    <mergeCell ref="C56:C64"/>
-    <mergeCell ref="C65:C73"/>
-    <mergeCell ref="C74:C82"/>
-    <mergeCell ref="C2:C9"/>
-    <mergeCell ref="C10:C17"/>
-    <mergeCell ref="C18:C25"/>
-    <mergeCell ref="C26:C33"/>
-    <mergeCell ref="C34:C41"/>
+    <mergeCell ref="A26:A33"/>
+    <mergeCell ref="A34:A41"/>
     <mergeCell ref="A42:A49"/>
     <mergeCell ref="A50:A55"/>
     <mergeCell ref="A56:A73"/>
@@ -6190,8 +6181,17 @@
     <mergeCell ref="A2:A9"/>
     <mergeCell ref="A10:A17"/>
     <mergeCell ref="A18:A25"/>
-    <mergeCell ref="A26:A33"/>
-    <mergeCell ref="A34:A41"/>
+    <mergeCell ref="C2:C9"/>
+    <mergeCell ref="C10:C17"/>
+    <mergeCell ref="C18:C25"/>
+    <mergeCell ref="C26:C33"/>
+    <mergeCell ref="C34:C41"/>
+    <mergeCell ref="C83:C97"/>
+    <mergeCell ref="C42:C49"/>
+    <mergeCell ref="C50:C55"/>
+    <mergeCell ref="C56:C64"/>
+    <mergeCell ref="C65:C73"/>
+    <mergeCell ref="C74:C82"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>